<commit_message>
organising, rerunning, adding new notebook on reweighting
</commit_message>
<xml_diff>
--- a/data/interim/wcss.xlsx
+++ b/data/interim/wcss.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjark/Documents/Python/clustering.nosync/data/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F7EED6BE-9DAD-5645-80DF-EC5234E8A0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA9482-88A1-F548-B8E0-3826547F4747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500"/>
+    <workbookView xWindow="28800" yWindow="-9000" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wcss" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">wcss!$B$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">wcss!$B$3:$B$51</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">wcss!$C$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">wcss!$C$3:$C$51</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">wcss!$B$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">wcss!$B$3:$B$51</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">wcss!$C$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">wcss!$C$3:$C$51</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -593,37 +596,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -644,9 +617,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="41275" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -967,7 +942,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E938-6248-B9D6-3807C5C65B41}"/>
@@ -993,6 +968,65 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t># of clusters</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1001,9 +1035,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="75000"/>
+                <a:alpha val="98000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1015,16 +1049,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-FR"/>
@@ -1035,30 +1066,77 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="4"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="353428352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3200"/>
           <c:min val="1400"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>total withinness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1075,16 +1153,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-FR"/>
@@ -1096,7 +1171,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1110,13 +1185,8 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+    <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1126,7 +1196,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-FR"/>
     </a:p>
@@ -1701,12 +1775,12 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>134099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457515</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
@@ -1731,6 +1805,150 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>315528</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>102547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323416</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>70994</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFB6508F-9666-B7F9-9EC9-150CB4BF208D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5285093" y="3794224"/>
+          <a:ext cx="7888" cy="2634658"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>307641</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>23665</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47330</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0EF2B7D-B869-02F3-0E48-5004959CE435}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5277206" y="5080001"/>
+          <a:ext cx="1372546" cy="504845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-FR"/>
+            <a:t>Withinness</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-FR" baseline="0"/>
+            <a:t> for </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-FR" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-FR" baseline="0"/>
+            <a:t>16 clusters: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-FR" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1796</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2032,11 +2250,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="249" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>